<commit_message>
Added normalized output columns.
</commit_message>
<xml_diff>
--- a/fuzzy/TestCases.xlsx
+++ b/fuzzy/TestCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>INPUT</t>
   </si>
@@ -56,18 +56,6 @@
     <t>Current FD %</t>
   </si>
   <si>
-    <t xml:space="preserve">Rec  Bond </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec Cash </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec  Fixed Deposit </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rec  Stock </t>
-  </si>
-  <si>
     <t>Property (0,1,2)</t>
   </si>
   <si>
@@ -96,6 +84,33 @@
   </si>
   <si>
     <t xml:space="preserve"> INTERMEDIATES  (0-2, 0=Decrease, 1=Maintain, 2=Increase)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final  Bond </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Cash </t>
+  </si>
+  <si>
+    <t>Final  FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final  Stock </t>
+  </si>
+  <si>
+    <t>NORMALIZED OUTPUT</t>
+  </si>
+  <si>
+    <t>Bond</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>FD</t>
+  </si>
+  <si>
+    <t>Stock</t>
   </si>
 </sst>
 </file>
@@ -133,7 +148,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -201,19 +216,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -278,11 +280,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -297,34 +379,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -339,6 +397,49 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -654,11 +755,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:Y33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K20" sqref="K20"/>
+      <selection pane="bottomLeft" activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -671,43 +772,49 @@
     <col min="6" max="6" width="20.21875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="8" max="14" width="15.109375" customWidth="1"/>
-    <col min="15" max="19" width="17.5546875" customWidth="1"/>
-    <col min="20" max="20" width="18.6640625" customWidth="1"/>
+    <col min="15" max="23" width="17.5546875" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="16" t="s">
+    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="10"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="12" t="s">
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="4" t="s">
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" s="7" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -729,226 +836,286 @@
       <c r="G2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="P2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="15" t="s">
+      <c r="Q2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="15" t="s">
+      <c r="R2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="U2" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="V2" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="29" t="s">
+        <v>28</v>
+      </c>
+      <c r="X2" s="25"/>
+      <c r="Y2" s="6"/>
+    </row>
+    <row r="3" spans="1:25" s="11" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>18</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="7"/>
-    </row>
-    <row r="3" spans="1:21" s="19" customFormat="1" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17">
+      <c r="B3" s="9">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="9">
+        <v>0</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+      <c r="F3" s="9">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>0</v>
+      </c>
+      <c r="H3" s="9">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>1</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0</v>
+      </c>
+      <c r="K3" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M3" s="9">
+        <v>1</v>
+      </c>
+      <c r="N3" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="O3" s="10">
+        <v>54.543999999999997</v>
+      </c>
+      <c r="P3" s="10">
+        <v>54.543999999999997</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="R3" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="S3" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="T3" s="26">
+        <f>O3/($O3+$P3+$Q3+$R3)</f>
+        <v>0.42857591853411697</v>
+      </c>
+      <c r="U3" s="26">
+        <f t="shared" ref="U3:W3" si="0">P3/($O3+$P3+$Q3+$R3)</f>
+        <v>0.42857591853411697</v>
+      </c>
+      <c r="V3" s="26">
+        <f t="shared" si="0"/>
+        <v>7.1424081465883013E-2</v>
+      </c>
+      <c r="W3" s="26">
+        <f t="shared" si="0"/>
+        <v>7.1424081465883013E-2</v>
+      </c>
+      <c r="X3" s="10"/>
+    </row>
+    <row r="4" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
         <v>18</v>
       </c>
-      <c r="B3" s="17">
-        <v>10000</v>
-      </c>
-      <c r="C3" s="17">
-        <v>0</v>
-      </c>
-      <c r="D3" s="17">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17">
-        <v>0</v>
-      </c>
-      <c r="F3" s="17">
-        <v>0</v>
-      </c>
-      <c r="G3" s="17">
-        <v>0</v>
-      </c>
-      <c r="H3" s="17">
-        <v>0</v>
-      </c>
-      <c r="I3" s="20">
+      <c r="B4" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C4" s="9">
+        <v>0</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0</v>
+      </c>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
+      <c r="F4" s="9">
+        <v>0</v>
+      </c>
+      <c r="G4" s="9">
+        <v>0</v>
+      </c>
+      <c r="H4" s="9">
+        <v>0</v>
+      </c>
+      <c r="I4" s="14">
+        <v>0.01</v>
+      </c>
+      <c r="J4" s="12">
+        <v>0.99</v>
+      </c>
+      <c r="K4" s="9">
         <v>1</v>
       </c>
-      <c r="J3" s="17">
-        <v>0</v>
-      </c>
-      <c r="K3" s="17">
+      <c r="L4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N4" s="9">
+        <v>1.49</v>
+      </c>
+      <c r="O4" s="10">
+        <v>16.565999999999999</v>
+      </c>
+      <c r="P4" s="10">
+        <v>54.545999999999999</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>9.09</v>
+      </c>
+      <c r="R4" s="10">
+        <v>54.088000000000001</v>
+      </c>
+      <c r="S4" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="T4" s="10">
+        <f t="shared" ref="T4:T21" si="1">O4/($O4+$P4+$Q4+$R4)</f>
+        <v>0.1233598927693797</v>
+      </c>
+      <c r="U4" s="10">
+        <f t="shared" ref="U4:U21" si="2">P4/($O4+$P4+$Q4+$R4)</f>
+        <v>0.40618065380892099</v>
+      </c>
+      <c r="V4" s="10">
+        <f t="shared" ref="V4:V21" si="3">Q4/($O4+$P4+$Q4+$R4)</f>
+        <v>6.7689329063966047E-2</v>
+      </c>
+      <c r="W4" s="10">
+        <f t="shared" ref="W4:W21" si="4">R4/($O4+$P4+$Q4+$R4)</f>
+        <v>0.40277012435773329</v>
+      </c>
+      <c r="X4" s="10"/>
+    </row>
+    <row r="5" spans="1:25" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>40</v>
+      </c>
+      <c r="B5" s="9">
+        <v>500000</v>
+      </c>
+      <c r="C5" s="9">
+        <v>0</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
+      <c r="F5" s="9">
+        <v>0</v>
+      </c>
+      <c r="G5" s="9">
+        <v>0</v>
+      </c>
+      <c r="H5" s="9">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0.81</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0</v>
+      </c>
+      <c r="K5" s="9">
         <v>1.5</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L5" s="9">
         <v>0.5</v>
       </c>
-      <c r="M3" s="17">
+      <c r="M5" s="9">
         <v>1</v>
       </c>
-      <c r="N3" s="17">
+      <c r="N5" s="9">
         <v>0.95</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O5" s="10">
         <v>54.543999999999997</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P5" s="10">
         <v>54.543999999999997</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q5" s="10">
         <v>9.09</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R5" s="10">
         <v>9.09</v>
       </c>
-      <c r="S3" s="18">
+      <c r="S5" s="10">
         <v>1.8</v>
       </c>
-      <c r="T3" s="18"/>
-    </row>
-    <row r="4" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="17">
-        <v>18</v>
-      </c>
-      <c r="B4" s="17">
-        <v>500000</v>
-      </c>
-      <c r="C4" s="17">
-        <v>0</v>
-      </c>
-      <c r="D4" s="17">
-        <v>0</v>
-      </c>
-      <c r="E4" s="17">
-        <v>0</v>
-      </c>
-      <c r="F4" s="17">
-        <v>0</v>
-      </c>
-      <c r="G4" s="17">
-        <v>0</v>
-      </c>
-      <c r="H4" s="17">
-        <v>0</v>
-      </c>
-      <c r="I4" s="22">
-        <v>0.01</v>
-      </c>
-      <c r="J4" s="20">
-        <v>0.99</v>
-      </c>
-      <c r="K4" s="17">
-        <v>1</v>
-      </c>
-      <c r="L4" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="M4" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="N4" s="17">
-        <v>1.49</v>
-      </c>
-      <c r="O4" s="18">
-        <v>16.565999999999999</v>
-      </c>
-      <c r="P4" s="18">
-        <v>54.545999999999999</v>
-      </c>
-      <c r="Q4" s="18">
-        <v>9.09</v>
-      </c>
-      <c r="R4" s="18">
-        <v>54.088000000000001</v>
-      </c>
-      <c r="S4" s="18">
-        <v>1.8</v>
-      </c>
-      <c r="T4" s="18"/>
-    </row>
-    <row r="5" spans="1:21" s="19" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="17">
-        <v>40</v>
-      </c>
-      <c r="B5" s="17">
-        <v>500000</v>
-      </c>
-      <c r="C5" s="17">
-        <v>0</v>
-      </c>
-      <c r="D5" s="17">
-        <v>0</v>
-      </c>
-      <c r="E5" s="17">
-        <v>0</v>
-      </c>
-      <c r="F5" s="17">
-        <v>0</v>
-      </c>
-      <c r="G5" s="17">
-        <v>0</v>
-      </c>
-      <c r="H5" s="17">
-        <v>0</v>
-      </c>
-      <c r="I5" s="20">
-        <v>0.81</v>
-      </c>
-      <c r="J5" s="17">
-        <v>0</v>
-      </c>
-      <c r="K5" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="L5" s="17">
-        <v>0.5</v>
-      </c>
-      <c r="M5" s="17">
-        <v>1</v>
-      </c>
-      <c r="N5" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="O5" s="18">
-        <v>54.543999999999997</v>
-      </c>
-      <c r="P5" s="18">
-        <v>54.543999999999997</v>
-      </c>
-      <c r="Q5" s="18">
-        <v>9.09</v>
-      </c>
-      <c r="R5" s="18">
-        <v>9.09</v>
-      </c>
-      <c r="S5" s="18">
-        <v>1.8</v>
-      </c>
-      <c r="T5" s="18"/>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T5" s="10">
+        <f t="shared" si="1"/>
+        <v>0.42857591853411697</v>
+      </c>
+      <c r="U5" s="10">
+        <f t="shared" si="2"/>
+        <v>0.42857591853411697</v>
+      </c>
+      <c r="V5" s="10">
+        <f t="shared" si="3"/>
+        <v>7.1424081465883013E-2</v>
+      </c>
+      <c r="W5" s="10">
+        <f t="shared" si="4"/>
+        <v>7.1424081465883013E-2</v>
+      </c>
+      <c r="X5" s="10"/>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>35</v>
       </c>
@@ -973,22 +1140,22 @@
       <c r="H6" s="2">
         <v>0</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="13">
         <v>0.63</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
       </c>
-      <c r="K6" s="17">
+      <c r="K6" s="9">
         <v>1.5</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="9">
         <v>1</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="9">
         <v>1</v>
       </c>
-      <c r="N6" s="17">
+      <c r="N6" s="9">
         <v>0.95</v>
       </c>
       <c r="O6" s="1">
@@ -1006,9 +1173,25 @@
       <c r="S6" s="1">
         <v>1</v>
       </c>
-      <c r="T6" s="1"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.66669111176298035</v>
+      </c>
+      <c r="U6" s="10">
+        <f t="shared" si="2"/>
+        <v>0.11110296274567322</v>
+      </c>
+      <c r="V6" s="10">
+        <f t="shared" si="3"/>
+        <v>0.11110296274567322</v>
+      </c>
+      <c r="W6" s="10">
+        <f t="shared" si="4"/>
+        <v>0.11110296274567322</v>
+      </c>
+      <c r="X6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>30</v>
       </c>
@@ -1033,7 +1216,7 @@
       <c r="H7" s="2">
         <v>0</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="13">
         <v>0.44</v>
       </c>
       <c r="J7" s="2">
@@ -1066,9 +1249,25 @@
       <c r="S7" s="1">
         <v>1.3186</v>
       </c>
-      <c r="T7" s="1"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T7" s="10">
+        <f t="shared" si="1"/>
+        <v>0.28748218137780529</v>
+      </c>
+      <c r="U7" s="10">
+        <f t="shared" si="2"/>
+        <v>0.26390483278878785</v>
+      </c>
+      <c r="V7" s="10">
+        <f t="shared" si="3"/>
+        <v>0.1374651511902209</v>
+      </c>
+      <c r="W7" s="10">
+        <f t="shared" si="4"/>
+        <v>0.31114783464318602</v>
+      </c>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>30</v>
       </c>
@@ -1090,7 +1289,7 @@
       <c r="G8" s="2">
         <v>0</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="13">
         <v>0.4</v>
       </c>
       <c r="I8" s="2">
@@ -1126,9 +1325,25 @@
       <c r="S8" s="1">
         <v>1.8</v>
       </c>
-      <c r="T8" s="1"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T8" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35869107744107742</v>
+      </c>
+      <c r="U8" s="10">
+        <f t="shared" si="2"/>
+        <v>0.35870422979797983</v>
+      </c>
+      <c r="V8" s="10">
+        <f t="shared" si="3"/>
+        <v>0.22282723063973064</v>
+      </c>
+      <c r="W8" s="10">
+        <f t="shared" si="4"/>
+        <v>5.977746212121212E-2</v>
+      </c>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>30</v>
       </c>
@@ -1150,7 +1365,7 @@
       <c r="G9" s="2">
         <v>0</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="13">
         <v>0.44</v>
       </c>
       <c r="I9" s="2">
@@ -1186,9 +1401,25 @@
       <c r="S9" s="1">
         <v>1.8</v>
       </c>
-      <c r="T9" s="1"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T9" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35275248344370858</v>
+      </c>
+      <c r="U9" s="10">
+        <f t="shared" si="2"/>
+        <v>0.35276541804635764</v>
+      </c>
+      <c r="V9" s="10">
+        <f t="shared" si="3"/>
+        <v>0.23569432947019869</v>
+      </c>
+      <c r="W9" s="10">
+        <f t="shared" si="4"/>
+        <v>5.8787769039735101E-2</v>
+      </c>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>30</v>
       </c>
@@ -1213,7 +1444,7 @@
       <c r="H10" s="2">
         <v>0</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="13">
         <v>0.44</v>
       </c>
       <c r="J10" s="2">
@@ -1246,9 +1477,25 @@
       <c r="S10" s="1">
         <v>1.3186</v>
       </c>
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35283334519826293</v>
+      </c>
+      <c r="U10" s="10">
+        <f t="shared" si="2"/>
+        <v>0.32430412187655727</v>
+      </c>
+      <c r="V10" s="10">
+        <f t="shared" si="3"/>
+        <v>8.0889157827294084E-2</v>
+      </c>
+      <c r="W10" s="10">
+        <f t="shared" si="4"/>
+        <v>0.24197337509788566</v>
+      </c>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>30</v>
       </c>
@@ -1273,7 +1520,7 @@
       <c r="H11" s="2">
         <v>0.09</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="13">
         <v>0.44</v>
       </c>
       <c r="J11" s="2">
@@ -1306,9 +1553,25 @@
       <c r="S11" s="1">
         <v>1.8</v>
       </c>
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T11" s="10">
+        <f t="shared" si="1"/>
+        <v>0.62651065465260269</v>
+      </c>
+      <c r="U11" s="10">
+        <f t="shared" si="2"/>
+        <v>0.17939958150061919</v>
+      </c>
+      <c r="V11" s="10">
+        <f t="shared" si="3"/>
+        <v>9.7044881923388976E-2</v>
+      </c>
+      <c r="W11" s="10">
+        <f t="shared" si="4"/>
+        <v>9.7044881923388976E-2</v>
+      </c>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>30</v>
       </c>
@@ -1333,7 +1596,7 @@
       <c r="H12" s="2">
         <v>0.09</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="13">
         <v>0.44</v>
       </c>
       <c r="J12" s="2">
@@ -1366,9 +1629,25 @@
       <c r="S12" s="1">
         <v>1.8</v>
       </c>
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T12" s="10">
+        <f t="shared" si="1"/>
+        <v>0.40407752029870203</v>
+      </c>
+      <c r="U12" s="10">
+        <f t="shared" si="2"/>
+        <v>0.12448882830557693</v>
+      </c>
+      <c r="V12" s="10">
+        <f t="shared" si="3"/>
+        <v>6.7341314526166055E-2</v>
+      </c>
+      <c r="W12" s="10">
+        <f t="shared" si="4"/>
+        <v>0.40409233686955487</v>
+      </c>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>45</v>
       </c>
@@ -1390,7 +1669,7 @@
       <c r="G13" s="2">
         <v>0</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="13">
         <v>0.4</v>
       </c>
       <c r="I13" s="2">
@@ -1426,9 +1705,25 @@
       <c r="S13" s="1">
         <v>1.6667000000000001</v>
       </c>
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T13" s="10">
+        <f t="shared" si="1"/>
+        <v>0.35869107744107742</v>
+      </c>
+      <c r="U13" s="10">
+        <f t="shared" si="2"/>
+        <v>0.35870422979797983</v>
+      </c>
+      <c r="V13" s="10">
+        <f t="shared" si="3"/>
+        <v>0.22282723063973064</v>
+      </c>
+      <c r="W13" s="10">
+        <f t="shared" si="4"/>
+        <v>5.977746212121212E-2</v>
+      </c>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>45</v>
       </c>
@@ -1450,7 +1745,7 @@
       <c r="G14" s="2">
         <v>0</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="13">
         <v>0.4</v>
       </c>
       <c r="I14" s="2">
@@ -1486,9 +1781,25 @@
       <c r="S14" s="1">
         <v>0.86670000000000003</v>
       </c>
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T14" s="10">
+        <f t="shared" si="1"/>
+        <v>0.5116313972684976</v>
+      </c>
+      <c r="U14" s="10">
+        <f t="shared" si="2"/>
+        <v>0.3178373105207864</v>
+      </c>
+      <c r="V14" s="10">
+        <f t="shared" si="3"/>
+        <v>8.5265646105357945E-2</v>
+      </c>
+      <c r="W14" s="10">
+        <f t="shared" si="4"/>
+        <v>8.5265646105357945E-2</v>
+      </c>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>45</v>
       </c>
@@ -1510,7 +1821,7 @@
       <c r="G15" s="2">
         <v>100</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="13">
         <v>0.82</v>
       </c>
       <c r="I15" s="2">
@@ -1546,9 +1857,25 @@
       <c r="S15" s="1">
         <v>1.6667000000000001</v>
       </c>
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="T15" s="10">
+        <f t="shared" si="1"/>
+        <v>0.3316592080941726</v>
+      </c>
+      <c r="U15" s="10">
+        <f t="shared" si="2"/>
+        <v>0.28141112948730418</v>
+      </c>
+      <c r="V15" s="10">
+        <f t="shared" si="3"/>
+        <v>5.5270454324350619E-2</v>
+      </c>
+      <c r="W15" s="10">
+        <f t="shared" si="4"/>
+        <v>0.3316592080941726</v>
+      </c>
+      <c r="X15" s="1"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>45</v>
       </c>
@@ -1573,7 +1900,7 @@
       <c r="H16" s="2">
         <v>0.2</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="13">
         <v>0.99</v>
       </c>
       <c r="J16" s="2">
@@ -1606,9 +1933,25 @@
       <c r="S16" s="1">
         <v>1.6667000000000001</v>
       </c>
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T16" s="10">
+        <f t="shared" si="1"/>
+        <v>0.40429916240456598</v>
+      </c>
+      <c r="U16" s="10">
+        <f t="shared" si="2"/>
+        <v>0.40431398710251282</v>
+      </c>
+      <c r="V16" s="10">
+        <f t="shared" si="3"/>
+        <v>0.12400859832480914</v>
+      </c>
+      <c r="W16" s="10">
+        <f t="shared" si="4"/>
+        <v>6.7378252168112079E-2</v>
+      </c>
+      <c r="X16" s="1"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>45</v>
       </c>
@@ -1633,7 +1976,7 @@
       <c r="H17" s="2">
         <v>0.2</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="13">
         <v>0.99</v>
       </c>
       <c r="J17" s="2">
@@ -1666,9 +2009,25 @@
       <c r="S17" s="1">
         <v>1.6667000000000001</v>
       </c>
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T17" s="10">
+        <f t="shared" si="1"/>
+        <v>0.33295892953069295</v>
+      </c>
+      <c r="U17" s="10">
+        <f t="shared" si="2"/>
+        <v>0.33297113835034425</v>
+      </c>
+      <c r="V17" s="10">
+        <f t="shared" si="3"/>
+        <v>5.5489085315231723E-2</v>
+      </c>
+      <c r="W17" s="10">
+        <f t="shared" si="4"/>
+        <v>0.27858084680373102</v>
+      </c>
+      <c r="X17" s="1"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>45</v>
       </c>
@@ -1693,7 +2052,7 @@
       <c r="H18" s="2">
         <v>0.2</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="13">
         <v>0.59</v>
       </c>
       <c r="J18" s="2">
@@ -1726,9 +2085,25 @@
       <c r="S18" s="1">
         <v>0.86670000000000003</v>
       </c>
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T18" s="10">
+        <f t="shared" si="1"/>
+        <v>0.58503153288429355</v>
+      </c>
+      <c r="U18" s="10">
+        <f t="shared" si="2"/>
+        <v>0.21997940709597152</v>
+      </c>
+      <c r="V18" s="10">
+        <f t="shared" si="3"/>
+        <v>9.7494530009867422E-2</v>
+      </c>
+      <c r="W18" s="10">
+        <f t="shared" si="4"/>
+        <v>9.7494530009867422E-2</v>
+      </c>
+      <c r="X18" s="1"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>65</v>
       </c>
@@ -1750,7 +2125,7 @@
       <c r="G19" s="2">
         <v>15</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="13">
         <v>0.8</v>
       </c>
       <c r="I19" s="2">
@@ -1786,9 +2161,25 @@
       <c r="S19" s="1">
         <v>1</v>
       </c>
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T19" s="10">
+        <f t="shared" si="1"/>
+        <v>0.37273124863328233</v>
+      </c>
+      <c r="U19" s="10">
+        <f t="shared" si="2"/>
+        <v>0.24400010933741531</v>
+      </c>
+      <c r="V19" s="10">
+        <f t="shared" si="3"/>
+        <v>0.19389623879291495</v>
+      </c>
+      <c r="W19" s="10">
+        <f t="shared" si="4"/>
+        <v>0.18937240323638752</v>
+      </c>
+      <c r="X19" s="1"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>65</v>
       </c>
@@ -1810,7 +2201,7 @@
       <c r="G20" s="2">
         <v>0</v>
       </c>
-      <c r="H20" s="21">
+      <c r="H20" s="13">
         <v>0.4</v>
       </c>
       <c r="I20" s="2">
@@ -1846,9 +2237,25 @@
       <c r="S20" s="1">
         <v>1</v>
       </c>
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T20" s="10">
+        <f t="shared" si="1"/>
+        <v>0.31578337945648016</v>
+      </c>
+      <c r="U20" s="10">
+        <f t="shared" si="2"/>
+        <v>0.31579495848916783</v>
+      </c>
+      <c r="V20" s="10">
+        <f t="shared" si="3"/>
+        <v>0.31579495848916783</v>
+      </c>
+      <c r="W20" s="10">
+        <f t="shared" si="4"/>
+        <v>5.2626703565184167E-2</v>
+      </c>
+      <c r="X20" s="1"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>65</v>
       </c>
@@ -1870,7 +2277,7 @@
       <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="H21" s="21">
+      <c r="H21" s="13">
         <v>0.8</v>
       </c>
       <c r="I21" s="2">
@@ -1906,9 +2313,25 @@
       <c r="S21" s="1">
         <v>0.2</v>
       </c>
-      <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T21" s="10">
+        <f t="shared" si="1"/>
+        <v>0.42856918362536334</v>
+      </c>
+      <c r="U21" s="10">
+        <f t="shared" si="2"/>
+        <v>0.42858489824781953</v>
+      </c>
+      <c r="V21" s="10">
+        <f t="shared" si="3"/>
+        <v>7.1422959063408495E-2</v>
+      </c>
+      <c r="W21" s="10">
+        <f t="shared" si="4"/>
+        <v>7.1422959063408495E-2</v>
+      </c>
+      <c r="X21" s="1"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1929,8 +2352,12 @@
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1951,8 +2378,12 @@
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1973,8 +2404,12 @@
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1995,8 +2430,12 @@
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2017,8 +2456,12 @@
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2039,8 +2482,12 @@
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2061,8 +2508,12 @@
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2083,8 +2534,12 @@
       <c r="R29" s="1"/>
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2105,8 +2560,12 @@
       <c r="R30" s="1"/>
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2127,8 +2586,12 @@
       <c r="R31" s="1"/>
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2149,8 +2612,12 @@
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+    </row>
+    <row r="33" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -2171,13 +2638,18 @@
       <c r="R33" s="1"/>
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="O1:S1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="H1:J1"/>
+    <mergeCell ref="T1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>